<commit_message>
updated files for disturbia.mp3
</commit_message>
<xml_diff>
--- a/Transition_Options.xlsx
+++ b/Transition_Options.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwise/Desktop/buildspace/streamlit_demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwise/Desktop/buildspace/automix_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96C2F54-9357-CF42-91A2-22D0834637B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52A919-D59E-D84D-9863-691D46CCACF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="500" windowWidth="21920" windowHeight="15120" activeTab="2" xr2:uid="{5E4F83DF-4589-A942-AC26-267E28EBCCB9}"/>
+    <workbookView xWindow="4960" yWindow="500" windowWidth="21920" windowHeight="15080" activeTab="1" xr2:uid="{5E4F83DF-4589-A942-AC26-267E28EBCCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Don't_Stop_The_Music.wav" sheetId="1" r:id="rId1"/>
-    <sheet name="Disturbia.wav" sheetId="2" r:id="rId2"/>
+    <sheet name="Disturbia.mp3" sheetId="2" r:id="rId2"/>
     <sheet name="Only_Girl.mp3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BB96B6-6C54-FF49-8845-BCA8276CE7BE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112BE76E-1014-C449-BDF9-AFB80E728A32}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>